<commit_message>
Add overall_end values for san diego state.
</commit_message>
<xml_diff>
--- a/data/datasets/roster_san_diego_state.xlsx
+++ b/data/datasets/roster_san_diego_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3916E31D-41E1-4255-AB79-88A20874335C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA4C8A5-95C9-4BC3-8BB9-14F9F42E03CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4586,8 +4586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4678,7 +4678,9 @@
       <c r="K2" s="2">
         <v>93</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -4714,7 +4716,9 @@
       <c r="K3" s="2">
         <v>86</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -4750,7 +4754,9 @@
       <c r="K4" s="2">
         <v>80</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -4786,7 +4792,9 @@
       <c r="K5" s="2">
         <v>78</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -4822,7 +4830,9 @@
       <c r="K6" s="3">
         <v>78</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3">
+        <v>78</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -4858,7 +4868,9 @@
       <c r="K7" s="2">
         <v>94</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -4894,7 +4906,9 @@
       <c r="K8" s="2">
         <v>82</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -4930,7 +4944,9 @@
       <c r="K9" s="2">
         <v>80</v>
       </c>
-      <c r="L9" s="2"/>
+      <c r="L9" s="2">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -4966,7 +4982,9 @@
       <c r="K10" s="2">
         <v>78</v>
       </c>
-      <c r="L10" s="2"/>
+      <c r="L10" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -5002,7 +5020,9 @@
       <c r="K11" s="3">
         <v>79</v>
       </c>
-      <c r="L11" s="3"/>
+      <c r="L11" s="3">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -5038,7 +5058,9 @@
       <c r="K12" s="3">
         <v>75</v>
       </c>
-      <c r="L12" s="3"/>
+      <c r="L12" s="3">
+        <v>75</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -5074,7 +5096,9 @@
       <c r="K13" s="2">
         <v>74</v>
       </c>
-      <c r="L13" s="2"/>
+      <c r="L13" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -5110,7 +5134,9 @@
       <c r="K14" s="2">
         <v>90</v>
       </c>
-      <c r="L14" s="2"/>
+      <c r="L14" s="2">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -5146,7 +5172,9 @@
       <c r="K15" s="2">
         <v>86</v>
       </c>
-      <c r="L15" s="2"/>
+      <c r="L15" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -5182,7 +5210,9 @@
       <c r="K16" s="2">
         <v>85</v>
       </c>
-      <c r="L16" s="2"/>
+      <c r="L16" s="2">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -5218,20 +5248,22 @@
       <c r="K17" s="2">
         <v>81</v>
       </c>
-      <c r="L17" s="2"/>
+      <c r="L17" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>248</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>249</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>52</v>
@@ -5249,25 +5281,27 @@
         <v>68</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K18" s="2">
-        <v>79</v>
-      </c>
-      <c r="L18" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="L18" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>248</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>249</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>52</v>
@@ -5285,12 +5319,14 @@
         <v>68</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K19" s="2">
-        <v>80</v>
-      </c>
-      <c r="L19" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="L19" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -5326,7 +5362,9 @@
       <c r="K20" s="2">
         <v>77</v>
       </c>
-      <c r="L20" s="2"/>
+      <c r="L20" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -5362,7 +5400,9 @@
       <c r="K21" s="2">
         <v>75</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -5398,7 +5438,9 @@
       <c r="K22" s="2">
         <v>75</v>
       </c>
-      <c r="L22" s="2"/>
+      <c r="L22" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -5434,7 +5476,9 @@
       <c r="K23" s="2">
         <v>73</v>
       </c>
-      <c r="L23" s="2"/>
+      <c r="L23" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -5470,7 +5514,9 @@
       <c r="K24" s="2">
         <v>83</v>
       </c>
-      <c r="L24" s="2"/>
+      <c r="L24" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -5506,7 +5552,9 @@
       <c r="K25" s="2">
         <v>84</v>
       </c>
-      <c r="L25" s="2"/>
+      <c r="L25" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -5542,7 +5590,9 @@
       <c r="K26" s="2">
         <v>76</v>
       </c>
-      <c r="L26" s="2"/>
+      <c r="L26" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -5578,7 +5628,9 @@
       <c r="K27" s="2">
         <v>74</v>
       </c>
-      <c r="L27" s="2"/>
+      <c r="L27" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -5614,7 +5666,9 @@
       <c r="K28" s="2">
         <v>73</v>
       </c>
-      <c r="L28" s="2"/>
+      <c r="L28" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -5650,7 +5704,9 @@
       <c r="K29" s="2">
         <v>88</v>
       </c>
-      <c r="L29" s="2"/>
+      <c r="L29" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -5686,7 +5742,9 @@
       <c r="K30" s="2">
         <v>80</v>
       </c>
-      <c r="L30" s="2"/>
+      <c r="L30" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -5722,7 +5780,9 @@
       <c r="K31" s="3">
         <v>69</v>
       </c>
-      <c r="L31" s="3"/>
+      <c r="L31" s="3">
+        <v>69</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -5758,7 +5818,9 @@
       <c r="K32" s="2">
         <v>86</v>
       </c>
-      <c r="L32" s="2"/>
+      <c r="L32" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -5794,7 +5856,9 @@
       <c r="K33" s="2">
         <v>82</v>
       </c>
-      <c r="L33" s="2"/>
+      <c r="L33" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -5830,7 +5894,9 @@
       <c r="K34" s="2">
         <v>68</v>
       </c>
-      <c r="L34" s="2"/>
+      <c r="L34" s="2">
+        <v>68</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -5866,7 +5932,9 @@
       <c r="K35" s="2">
         <v>89</v>
       </c>
-      <c r="L35" s="2"/>
+      <c r="L35" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -5902,7 +5970,9 @@
       <c r="K36" s="2">
         <v>80</v>
       </c>
-      <c r="L36" s="2"/>
+      <c r="L36" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -5938,7 +6008,9 @@
       <c r="K37" s="2">
         <v>83</v>
       </c>
-      <c r="L37" s="2"/>
+      <c r="L37" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -5974,7 +6046,9 @@
       <c r="K38" s="2">
         <v>77</v>
       </c>
-      <c r="L38" s="2"/>
+      <c r="L38" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -6010,7 +6084,9 @@
       <c r="K39" s="3">
         <v>76</v>
       </c>
-      <c r="L39" s="3"/>
+      <c r="L39" s="3">
+        <v>76</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -6046,7 +6122,9 @@
       <c r="K40" s="2">
         <v>91</v>
       </c>
-      <c r="L40" s="2"/>
+      <c r="L40" s="2">
+        <v>92</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -6082,7 +6160,9 @@
       <c r="K41" s="2">
         <v>85</v>
       </c>
-      <c r="L41" s="2"/>
+      <c r="L41" s="2">
+        <v>85</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -6118,7 +6198,9 @@
       <c r="K42" s="2">
         <v>79</v>
       </c>
-      <c r="L42" s="2"/>
+      <c r="L42" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -6154,7 +6236,9 @@
       <c r="K43" s="2">
         <v>78</v>
       </c>
-      <c r="L43" s="2"/>
+      <c r="L43" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -6190,7 +6274,9 @@
       <c r="K44" s="2">
         <v>77</v>
       </c>
-      <c r="L44" s="2"/>
+      <c r="L44" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -6226,7 +6312,9 @@
       <c r="K45" s="2">
         <v>86</v>
       </c>
-      <c r="L45" s="2"/>
+      <c r="L45" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -6262,7 +6350,9 @@
       <c r="K46" s="2">
         <v>78</v>
       </c>
-      <c r="L46" s="2"/>
+      <c r="L46" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -6298,7 +6388,9 @@
       <c r="K47" s="2">
         <v>78</v>
       </c>
-      <c r="L47" s="2"/>
+      <c r="L47" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -6334,7 +6426,9 @@
       <c r="K48" s="2">
         <v>72</v>
       </c>
-      <c r="L48" s="2"/>
+      <c r="L48" s="2">
+        <v>72</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
@@ -6370,7 +6464,9 @@
       <c r="K49" s="2">
         <v>86</v>
       </c>
-      <c r="L49" s="2"/>
+      <c r="L49" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
@@ -6406,7 +6502,9 @@
       <c r="K50" s="3">
         <v>85</v>
       </c>
-      <c r="L50" s="3"/>
+      <c r="L50" s="3">
+        <v>85</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -6442,7 +6540,9 @@
       <c r="K51" s="3">
         <v>75</v>
       </c>
-      <c r="L51" s="3"/>
+      <c r="L51" s="3">
+        <v>75</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
@@ -6478,7 +6578,9 @@
       <c r="K52" s="2">
         <v>86</v>
       </c>
-      <c r="L52" s="2"/>
+      <c r="L52" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
@@ -6514,7 +6616,9 @@
       <c r="K53" s="2">
         <v>84</v>
       </c>
-      <c r="L53" s="2"/>
+      <c r="L53" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
@@ -6550,7 +6654,9 @@
       <c r="K54" s="2">
         <v>80</v>
       </c>
-      <c r="L54" s="2"/>
+      <c r="L54" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
@@ -6586,7 +6692,9 @@
       <c r="K55" s="2">
         <v>78</v>
       </c>
-      <c r="L55" s="2"/>
+      <c r="L55" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -6622,7 +6730,9 @@
       <c r="K56" s="2">
         <v>73</v>
       </c>
-      <c r="L56" s="2"/>
+      <c r="L56" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
@@ -6658,7 +6768,9 @@
       <c r="K57" s="2">
         <v>84</v>
       </c>
-      <c r="L57" s="2"/>
+      <c r="L57" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
@@ -6694,7 +6806,9 @@
       <c r="K58" s="2">
         <v>80</v>
       </c>
-      <c r="L58" s="2"/>
+      <c r="L58" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
@@ -6730,7 +6844,9 @@
       <c r="K59" s="2">
         <v>78</v>
       </c>
-      <c r="L59" s="2"/>
+      <c r="L59" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -6766,7 +6882,9 @@
       <c r="K60" s="3">
         <v>70</v>
       </c>
-      <c r="L60" s="3"/>
+      <c r="L60" s="3">
+        <v>70</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
@@ -6802,7 +6920,9 @@
       <c r="K61" s="2">
         <v>91</v>
       </c>
-      <c r="L61" s="2"/>
+      <c r="L61" s="2">
+        <v>94</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
@@ -6838,7 +6958,9 @@
       <c r="K62" s="2">
         <v>80</v>
       </c>
-      <c r="L62" s="2"/>
+      <c r="L62" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
@@ -6874,7 +6996,9 @@
       <c r="K63" s="2">
         <v>78</v>
       </c>
-      <c r="L63" s="2"/>
+      <c r="L63" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -6910,7 +7034,9 @@
       <c r="K64" s="3">
         <v>74</v>
       </c>
-      <c r="L64" s="3"/>
+      <c r="L64" s="3">
+        <v>74</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
@@ -6946,7 +7072,9 @@
       <c r="K65" s="2">
         <v>92</v>
       </c>
-      <c r="L65" s="2"/>
+      <c r="L65" s="2">
+        <v>92</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
@@ -6982,7 +7110,9 @@
       <c r="K66" s="2">
         <v>89</v>
       </c>
-      <c r="L66" s="2"/>
+      <c r="L66" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
@@ -7018,7 +7148,9 @@
       <c r="K67" s="2">
         <v>79</v>
       </c>
-      <c r="L67" s="2"/>
+      <c r="L67" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
@@ -7054,7 +7186,9 @@
       <c r="K68" s="2">
         <v>74</v>
       </c>
-      <c r="L68" s="2"/>
+      <c r="L68" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
@@ -7090,7 +7224,9 @@
       <c r="K69" s="2">
         <v>73</v>
       </c>
-      <c r="L69" s="2"/>
+      <c r="L69" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
@@ -7126,7 +7262,9 @@
       <c r="K70" s="2">
         <v>85</v>
       </c>
-      <c r="L70" s="2"/>
+      <c r="L70" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -7162,7 +7300,9 @@
       <c r="K71" s="2">
         <v>83</v>
       </c>
-      <c r="L71" s="2"/>
+      <c r="L71" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
@@ -7198,7 +7338,9 @@
       <c r="K72" s="2">
         <v>83</v>
       </c>
-      <c r="L72" s="2"/>
+      <c r="L72" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
@@ -7234,7 +7376,9 @@
       <c r="K73" s="2">
         <v>81</v>
       </c>
-      <c r="L73" s="2"/>
+      <c r="L73" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -7270,7 +7414,9 @@
       <c r="K74" s="2">
         <v>80</v>
       </c>
-      <c r="L74" s="2"/>
+      <c r="L74" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -7306,7 +7452,9 @@
       <c r="K75" s="2">
         <v>78</v>
       </c>
-      <c r="L75" s="2"/>
+      <c r="L75" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
@@ -7342,7 +7490,9 @@
       <c r="K76" s="2">
         <v>77</v>
       </c>
-      <c r="L76" s="2"/>
+      <c r="L76" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -7378,7 +7528,9 @@
       <c r="K77" s="2">
         <v>70</v>
       </c>
-      <c r="L77" s="2"/>
+      <c r="L77" s="2">
+        <v>70</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
@@ -7414,7 +7566,9 @@
       <c r="K78" s="2">
         <v>85</v>
       </c>
-      <c r="L78" s="2"/>
+      <c r="L78" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
@@ -7450,7 +7604,9 @@
       <c r="K79" s="2">
         <v>80</v>
       </c>
-      <c r="L79" s="2"/>
+      <c r="L79" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
@@ -7486,7 +7642,9 @@
       <c r="K80" s="2">
         <v>66</v>
       </c>
-      <c r="L80" s="2"/>
+      <c r="L80" s="2">
+        <v>66</v>
+      </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
@@ -7522,7 +7680,9 @@
       <c r="K81" s="2">
         <v>87</v>
       </c>
-      <c r="L81" s="2"/>
+      <c r="L81" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
@@ -7558,7 +7718,9 @@
       <c r="K82" s="2">
         <v>80</v>
       </c>
-      <c r="L82" s="2"/>
+      <c r="L82" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
@@ -7594,7 +7756,9 @@
       <c r="K83" s="2">
         <v>79</v>
       </c>
-      <c r="L83" s="2"/>
+      <c r="L83" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -7630,7 +7794,9 @@
       <c r="K84" s="2">
         <v>78</v>
       </c>
-      <c r="L84" s="2"/>
+      <c r="L84" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
@@ -7666,7 +7832,9 @@
       <c r="K85" s="2">
         <v>78</v>
       </c>
-      <c r="L85" s="2"/>
+      <c r="L85" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
@@ -7702,7 +7870,9 @@
       <c r="K86" s="2">
         <v>78</v>
       </c>
-      <c r="L86" s="2"/>
+      <c r="L86" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>

</xml_diff>